<commit_message>
Revert "Adding test script"
This reverts commit cea121d49b5389a285f2edfbe4a2065989a48f8d.
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/doctortestScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/doctortestScriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="6495" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="6495" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
@@ -12,8 +12,6 @@
     <sheet name="product" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="Doctor_Module" sheetId="5" r:id="rId5"/>
-    <sheet name="BookPatAppointment" sheetId="6" r:id="rId6"/>
-    <sheet name="AddingMedicalHistory" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="155">
   <si>
     <t>TC_ID</t>
   </si>
@@ -490,85 +488,19 @@
   </si>
   <si>
     <t>9789654321</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>DoctorSpecialization</t>
-  </si>
-  <si>
-    <t>DoctorName</t>
-  </si>
-  <si>
-    <t>Kani</t>
-  </si>
-  <si>
-    <t>BloodPressure</t>
-  </si>
-  <si>
-    <t>BloodSugar</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>BodyTemperature</t>
-  </si>
-  <si>
-    <t>Prescription</t>
-  </si>
-  <si>
-    <t>97/67</t>
-  </si>
-  <si>
-    <t>Nil</t>
-  </si>
-  <si>
-    <t>sona</t>
-  </si>
-  <si>
-    <t>7896543218</t>
-  </si>
-  <si>
-    <t>sona_</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>ch</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>Cardiology12</t>
-  </si>
-  <si>
-    <t>mani-28904684</t>
-  </si>
-  <si>
-    <t>45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF5B5B60"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -635,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -645,7 +577,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,7 +849,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1324,7 +1255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1295,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1303,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -2051,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,133 +2050,11 @@
       <c r="F3" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>155</v>
+      <c r="G3">
+        <v>30</v>
       </c>
       <c r="H3" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="H4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Adding test script""
This reverts commit ded53576b5b6ce916fdb2ff5d601292c5d4fc55e.
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/doctortestScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/doctortestScriptdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="6495" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15300" windowHeight="6495" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="product" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="Doctor_Module" sheetId="5" r:id="rId5"/>
+    <sheet name="BookPatAppointment" sheetId="6" r:id="rId6"/>
+    <sheet name="AddingMedicalHistory" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="175">
   <si>
     <t>TC_ID</t>
   </si>
@@ -488,19 +490,85 @@
   </si>
   <si>
     <t>9789654321</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>DoctorSpecialization</t>
+  </si>
+  <si>
+    <t>DoctorName</t>
+  </si>
+  <si>
+    <t>Kani</t>
+  </si>
+  <si>
+    <t>BloodPressure</t>
+  </si>
+  <si>
+    <t>BloodSugar</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>BodyTemperature</t>
+  </si>
+  <si>
+    <t>Prescription</t>
+  </si>
+  <si>
+    <t>97/67</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>sona</t>
+  </si>
+  <si>
+    <t>7896543218</t>
+  </si>
+  <si>
+    <t>sona_</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Cardiology12</t>
+  </si>
+  <si>
+    <t>mani-28904684</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF5B5B60"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -567,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -577,6 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,7 +918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1255,7 +1324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1271,7 +1340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1279,7 +1348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1295,7 +1364,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1303,7 +1372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1982,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,11 +2119,133 @@
       <c r="F3" t="s">
         <v>152</v>
       </c>
-      <c r="G3">
-        <v>30</v>
+      <c r="G3" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="H3" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>